<commit_message>
added demographics in Data.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Data.xlsx
+++ b/Documentation/Data.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Desktop\IBMDESC-Poverty\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renzo\Desktop\IBMDESC-Poverty\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="reference" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Region</t>
   </si>
@@ -147,6 +148,63 @@
   </si>
   <si>
     <t>Demographics</t>
+  </si>
+  <si>
+    <t>236.06 sq mi</t>
+  </si>
+  <si>
+    <t>5,024.19 sq mi</t>
+  </si>
+  <si>
+    <t>7,498.89 sq mi</t>
+  </si>
+  <si>
+    <t>10,899.21 sq mi</t>
+  </si>
+  <si>
+    <t>8,499.90 sq mi</t>
+  </si>
+  <si>
+    <t>6,514.82 sq mi</t>
+  </si>
+  <si>
+    <t>11,436.69 sq mi</t>
+  </si>
+  <si>
+    <t>7,010.00 sq mi</t>
+  </si>
+  <si>
+    <t>4,953.29 sq mi</t>
+  </si>
+  <si>
+    <t>5,154.75 sq mi</t>
+  </si>
+  <si>
+    <t>3,900.47 sq mi</t>
+  </si>
+  <si>
+    <t>8,977.30 sq mi</t>
+  </si>
+  <si>
+    <t>6,585.64 sq mi</t>
+  </si>
+  <si>
+    <t>7,913.56 sq mi</t>
+  </si>
+  <si>
+    <t>7,860.04 sq mi)</t>
+  </si>
+  <si>
+    <t>8,692.43 sq mi</t>
+  </si>
+  <si>
+    <t>8,292.84 sq mi</t>
+  </si>
+  <si>
+    <t>4,840.10 sq mi</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Regions_of_the_Philippines</t>
   </si>
 </sst>
 </file>
@@ -156,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +236,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,20 +281,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -543,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +624,7 @@
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
   </cols>
@@ -577,255 +649,327 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>12315437</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>2917</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>4874400</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>375</v>
       </c>
+      <c r="E3" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1676617</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>1105</v>
       </c>
+      <c r="E4" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>3325919</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>771</v>
       </c>
+      <c r="E5" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>10609616</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6">
         <v>2386</v>
       </c>
+      <c r="E6" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>13458967</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="6">
         <v>3082</v>
       </c>
+      <c r="E7" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2851028</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6">
         <v>638</v>
       </c>
+      <c r="E8" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>5591911</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="6">
         <v>1165</v>
       </c>
+      <c r="E9" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>7309153</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="6">
         <v>1604</v>
       </c>
+      <c r="E10" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>7060903</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="6">
         <v>1577</v>
       </c>
+      <c r="E12" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>4214633</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="6">
         <v>902</v>
       </c>
+      <c r="E13" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>3545610</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="6">
         <v>772</v>
       </c>
+      <c r="E14" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>4489614</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="6">
         <v>976</v>
       </c>
+      <c r="E15" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>4660027</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="6">
         <v>1078</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>4330622</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="6">
         <v>988</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E17" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>2507410</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="6">
         <v>532</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E18" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>3362501</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="6">
         <v>557</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated data and draft of final document
</commit_message>
<xml_diff>
--- a/Documentation/Data.xlsx
+++ b/Documentation/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Region</t>
   </si>
@@ -306,6 +306,9 @@
       </rPr>
       <t>Retrieved from https://www.philhealth.gov.ph/circulars/2001/circ21_2001.pdf</t>
     </r>
+  </si>
+  <si>
+    <t>Total Income of families (millions)</t>
   </si>
 </sst>
 </file>
@@ -728,11 +731,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,13 +746,13 @@
     <col min="4" max="4" width="34.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="28.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -772,16 +775,19 @@
         <v>57</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -804,16 +810,19 @@
         <v>2.6</v>
       </c>
       <c r="H2" s="9">
+        <v>1106169</v>
+      </c>
+      <c r="I2" s="9">
         <v>379</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>325</v>
       </c>
-      <c r="J2" s="9">
+      <c r="K2" s="9">
         <v>20344</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -836,16 +845,19 @@
         <v>14</v>
       </c>
       <c r="H3" s="9">
+        <v>225050</v>
+      </c>
+      <c r="I3" s="9">
         <v>204</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>159</v>
       </c>
-      <c r="J3" s="9">
+      <c r="K3" s="9">
         <v>18373</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -868,16 +880,19 @@
         <v>17.5</v>
       </c>
       <c r="H4" s="9">
+        <v>96351</v>
+      </c>
+      <c r="I4" s="9">
         <v>257</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>188</v>
       </c>
-      <c r="J4" s="9">
+      <c r="K4" s="9">
         <v>19483</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -900,16 +915,19 @@
         <v>17</v>
       </c>
       <c r="H5" s="9">
+        <v>150089</v>
+      </c>
+      <c r="I5" s="9">
         <v>195</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>140</v>
       </c>
-      <c r="J5" s="9">
+      <c r="K5" s="9">
         <v>19125</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -932,16 +950,19 @@
         <v>10.1</v>
       </c>
       <c r="H6" s="9">
+        <v>618893</v>
+      </c>
+      <c r="I6" s="9">
         <v>259</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>211</v>
       </c>
-      <c r="J6" s="9">
+      <c r="K6" s="9">
         <v>20071</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -964,16 +985,19 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="H7" s="9">
+        <v>876006</v>
+      </c>
+      <c r="I7" s="9">
         <v>284</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>243</v>
       </c>
-      <c r="J7" s="9">
+      <c r="K7" s="9">
         <v>19137</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -996,16 +1020,19 @@
         <v>23.6</v>
       </c>
       <c r="H8" s="9">
+        <v>114117</v>
+      </c>
+      <c r="I8" s="9">
         <v>179</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>138</v>
       </c>
-      <c r="J8" s="9">
+      <c r="K8" s="9">
         <v>17292</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1028,16 +1055,19 @@
         <v>32.299999999999997</v>
       </c>
       <c r="H9" s="9">
+        <v>189185</v>
+      </c>
+      <c r="I9" s="9">
         <v>162</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>144</v>
       </c>
-      <c r="J9" s="9">
+      <c r="K9" s="9">
         <v>18257</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -1060,16 +1090,19 @@
         <v>22.8</v>
       </c>
       <c r="H10" s="9">
+        <v>324028</v>
+      </c>
+      <c r="I10" s="9">
         <v>202</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>163</v>
       </c>
-      <c r="J10" s="9">
+      <c r="K10" s="9">
         <v>18029</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -1092,16 +1125,19 @@
         <v>25.7</v>
       </c>
       <c r="H11" s="9">
+        <v>329415</v>
+      </c>
+      <c r="I11" s="9">
         <v>209</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>164</v>
       </c>
-      <c r="J11" s="9">
+      <c r="K11" s="9">
         <v>18767</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -1124,16 +1160,19 @@
         <v>37.4</v>
       </c>
       <c r="H12" s="9">
+        <v>149493</v>
+      </c>
+      <c r="I12" s="9">
         <v>166</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>132</v>
       </c>
-      <c r="J12" s="9">
+      <c r="K12" s="9">
         <v>18076</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1156,16 +1195,19 @@
         <v>33.700000000000003</v>
       </c>
       <c r="H13" s="9">
+        <v>124903</v>
+      </c>
+      <c r="I13" s="9">
         <v>162</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>122</v>
       </c>
-      <c r="J13" s="9">
+      <c r="K13" s="9">
         <v>18054</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -1188,16 +1230,19 @@
         <v>32.799999999999997</v>
       </c>
       <c r="H14" s="9">
+        <v>185015</v>
+      </c>
+      <c r="I14" s="9">
         <v>190</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>143</v>
       </c>
-      <c r="J14" s="9">
+      <c r="K14" s="9">
         <v>19335</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1220,16 +1265,19 @@
         <v>25</v>
       </c>
       <c r="H15" s="9">
+        <v>209405</v>
+      </c>
+      <c r="I15" s="9">
         <v>194</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>156</v>
       </c>
-      <c r="J15" s="9">
+      <c r="K15" s="9">
         <v>19967</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
@@ -1252,16 +1300,19 @@
         <v>37.1</v>
       </c>
       <c r="H16" s="9">
+        <v>160674</v>
+      </c>
+      <c r="I16" s="9">
         <v>163</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>140</v>
       </c>
-      <c r="J16" s="9">
+      <c r="K16" s="9">
         <v>18737</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
@@ -1284,16 +1335,19 @@
         <v>31.9</v>
       </c>
       <c r="H17" s="9">
+        <v>95809</v>
+      </c>
+      <c r="I17" s="9">
         <v>180</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>142</v>
       </c>
-      <c r="J17" s="9">
+      <c r="K17" s="9">
         <v>19629</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1316,12 +1370,15 @@
         <v>48.7</v>
       </c>
       <c r="H18" s="9">
+        <v>72196</v>
+      </c>
+      <c r="I18" s="9">
         <v>130</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>114</v>
       </c>
-      <c r="J18" s="9">
+      <c r="K18" s="9">
         <v>20517</v>
       </c>
     </row>
@@ -1335,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>